<commit_message>
Added 10 mockup tweets
</commit_message>
<xml_diff>
--- a/Data/MockUP.xlsx
+++ b/Data/MockUP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesolis/Dropbox/local/local-doc/local-doc-edu/programming/BCTM/data-analist-bootcamp/Final_Project/Bootcamp_Final_Project/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luzhernandez/Desktop/Data Analysis/Projecto Final/Bootcamp_Final_Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E235155-68C6-9045-BFEC-6BC6717C783A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAF5C76-AE9C-0248-9ECB-968AF5AA03E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29460" yWindow="580" windowWidth="20240" windowHeight="19300" xr2:uid="{D65BEECF-CF03-E749-90E6-F98D29661669}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{D65BEECF-CF03-E749-90E6-F98D29661669}"/>
   </bookViews>
   <sheets>
     <sheet name="MockUP" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Loacation</t>
   </si>
@@ -104,6 +104,56 @@
   </si>
   <si>
     <t>Like</t>
+  </si>
+  <si>
+    <t>Hoy salió el Índice de Democracia 2021 de @TheEconomist.
+México ya no es considerado ni siquiera un país con una democracia defectuosa. Los puntajes ya nos colocan como un régimen híbrido, en camino al autoritarismo.
+Este mapa debería ser un escándalo.</t>
+  </si>
+  <si>
+    <t>El Gobierno de #España rechaza tajantemente las descalificaciones realizadas por el Presidente de #México, Andrés López Obrador. 
+México es un socio estratégico para nuestro país, y el Gobierno Bandera de España  desea unas relaciones basadas en el respeto mutuo.
+https://bit.ly/3GGmNJA</t>
+  </si>
+  <si>
+    <t>Donovan Carrillo Bandera de México trains alongside mostly teenagers in a shopping mall rink in León, Mexico, that is not Olympic size. It took a day to adjust his #Beijing2022 program. 
+Now he's made Olympic history, and he says you'll see him again in 2026. https://nyti.ms/3uDeQCx</t>
+  </si>
+  <si>
+    <t>De acuerdon con un análisis de The Economist, el sistema de salud está en colapso en México. El sistema tiene escasos médicos, enfermeras y camas de hospital y el 41 % del gasto en salud proviene del propio bolsillo, la proporción más alta en la OCDE.</t>
+  </si>
+  <si>
+    <t>Jalisco</t>
+  </si>
+  <si>
+    <t>The “Boy heroes”were six Mexican military cadets who were killed in the defence of Mexico City during the Battle of Chapultepec. Even though outnumbered &amp; ordered to retreat the six cadets refused to fall back and fought to the death. They were aged between 13-20.</t>
+  </si>
+  <si>
+    <t>Yucatan</t>
+  </si>
+  <si>
+    <t>Chichen Itza, one of the 7 wonders of the world is a complex of Mayan ruins centrally located on the northern half of Mexico’s Yucatan Peninsula. 
+📸 - Kriszti
+#mexico #yucatan</t>
+  </si>
+  <si>
+    <t>We want to ask you for a Valentine's card with the name "Liam Payne México" thank you @LiamPayne 💌💘🇲🇽 #HeresToTheFuture</t>
+  </si>
+  <si>
+    <t>Journalists in Mexico are posting a blank image as a protest against the killing of five journalists in 2022. #JournalismAtRisk</t>
+  </si>
+  <si>
+    <t>San Luis Potosi</t>
+  </si>
+  <si>
+    <t>Imagine if we were doing military drills a couple hundred miles from the Mexican border so China decided to say we were invading Mexico, and sent thousands of troops to the Guatemalan border.
+What would be our reaction?</t>
+  </si>
+  <si>
+    <t>Baja California</t>
+  </si>
+  <si>
+    <t>New Mexico StatePolice officer who was shot is in stable condition. Heavy police presence in the area, the scene is still very active. Suspects are still at large. Here are images from the scene just east of #Albquerque, #NewMexico @ABQJournal follow @MReisen88  for updates</t>
   </si>
 </sst>
 </file>
@@ -523,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CDB79B-AABF-2F46-9FC5-C3D5B57F6CF9}">
-  <dimension ref="B1:G11"/>
+  <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,6 +806,206 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="2:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>60</v>
+      </c>
+      <c r="E12" s="4">
+        <v>44602</v>
+      </c>
+      <c r="F12">
+        <v>2904</v>
+      </c>
+      <c r="G12">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13" s="4">
+        <v>44602</v>
+      </c>
+      <c r="F13">
+        <v>800</v>
+      </c>
+      <c r="G13">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4">
+        <v>44602</v>
+      </c>
+      <c r="F14">
+        <v>2142</v>
+      </c>
+      <c r="G14">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>27</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15">
+        <v>3000</v>
+      </c>
+      <c r="G15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>28</v>
+      </c>
+      <c r="E16" s="4">
+        <v>44239</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>47</v>
+      </c>
+      <c r="E17" s="4">
+        <v>44474</v>
+      </c>
+      <c r="F17">
+        <v>1000</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18" s="4">
+        <v>44572</v>
+      </c>
+      <c r="F18">
+        <v>2000</v>
+      </c>
+      <c r="G18">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="E19" s="4">
+        <v>44456</v>
+      </c>
+      <c r="F19">
+        <v>10000</v>
+      </c>
+      <c r="G19">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>33</v>
+      </c>
+      <c r="E20" s="4">
+        <v>44564</v>
+      </c>
+      <c r="F20">
+        <v>3000</v>
+      </c>
+      <c r="G20">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>53</v>
+      </c>
+      <c r="E21" s="4">
+        <v>44542</v>
+      </c>
+      <c r="F21">
+        <v>300</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>